<commit_message>
Final commit to project!
</commit_message>
<xml_diff>
--- a/automation/excel-outputs/FormErrorMessages.xlsx
+++ b/automation/excel-outputs/FormErrorMessages.xlsx
@@ -2,21 +2,21 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView windowHeight="6615" windowWidth="14715" xWindow="0" yWindow="2445"/>
   </bookViews>
   <sheets>
-    <sheet name="ChromeOutput" sheetId="1" r:id="rId1"/>
-    <sheet name="OperaOutput" sheetId="2" r:id="rId2"/>
-    <sheet name="FirefoxOutput" sheetId="3" r:id="rId3"/>
+    <sheet name="ChromeOutput" r:id="rId1" sheetId="1"/>
+    <sheet name="OperaOutput" r:id="rId2" sheetId="2"/>
+    <sheet name="FirefoxOutput" r:id="rId3" sheetId="3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="58">
   <si>
     <t>Sl no.</t>
   </si>
@@ -191,13 +191,14 @@
     <t>19</t>
   </si>
   <si>
-    <t>20</t>
+    <t>1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -252,27 +253,27 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="1" fillId="2" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Input" xfId="1" builtinId="20"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="20" name="Input" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium9" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -286,10 +287,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -447,7 +448,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -456,13 +457,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -472,7 +473,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -481,7 +482,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -490,7 +491,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -500,12 +501,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -536,7 +537,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -555,7 +556,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -567,25 +568,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="39.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="37.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="47" style="2" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18" style="2" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="9.140625" style="2" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="2" width="7.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="39.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="16.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="37.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="2" width="47.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="2" width="18.0" collapsed="true"/>
+    <col min="7" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row ht="45" r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -606,8 +607,8 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>1</v>
+      <c r="A2" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -630,13 +631,13 @@
         <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -650,16 +651,16 @@
         <v>40</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F4" t="s">
         <v>10</v>
@@ -670,7 +671,7 @@
         <v>41</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -690,16 +691,16 @@
         <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F6" t="s">
         <v>10</v>
@@ -710,16 +711,16 @@
         <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="F7" t="s">
         <v>10</v>
@@ -730,19 +731,19 @@
         <v>44</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E8" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F8" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -870,19 +871,19 @@
         <v>51</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E15" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F15" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -890,16 +891,16 @@
         <v>52</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>
       </c>
       <c r="D16" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E16" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="F16" t="s">
         <v>10</v>
@@ -910,13 +911,13 @@
         <v>53</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C17" t="s">
         <v>7</v>
       </c>
       <c r="D17" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E17" t="s">
         <v>9</v>
@@ -930,13 +931,13 @@
         <v>54</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C18" t="s">
         <v>7</v>
       </c>
       <c r="D18" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E18" t="s">
         <v>9</v>
@@ -950,13 +951,13 @@
         <v>55</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C19" t="s">
         <v>7</v>
       </c>
       <c r="D19" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E19" t="s">
         <v>9</v>
@@ -970,13 +971,13 @@
         <v>56</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C20" t="s">
         <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E20" t="s">
         <v>9</v>
@@ -986,50 +987,38 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>57</v>
-      </c>
-      <c r="B21" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" t="s">
-        <v>38</v>
-      </c>
-      <c r="E21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" t="s">
-        <v>10</v>
-      </c>
+      <c r="A21"/>
+      <c r="B21"/>
+      <c r="C21"/>
+      <c r="D21"/>
+      <c r="E21"/>
+      <c r="F21"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="A1:XFD1048576"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="39.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="37.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="47" style="2" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18" style="2" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="9.140625" style="2" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="2" width="7.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="39.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="16.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="37.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="2" width="47.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="2" width="18.0" collapsed="true"/>
+    <col min="7" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row ht="45" r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1050,8 +1039,8 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>1</v>
+      <c r="A2" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -1074,13 +1063,13 @@
         <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -1094,16 +1083,16 @@
         <v>40</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F4" t="s">
         <v>10</v>
@@ -1114,7 +1103,7 @@
         <v>41</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -1134,16 +1123,16 @@
         <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F6" t="s">
         <v>10</v>
@@ -1154,16 +1143,16 @@
         <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="F7" t="s">
         <v>10</v>
@@ -1174,19 +1163,19 @@
         <v>44</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E8" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F8" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1314,19 +1303,19 @@
         <v>51</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E15" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F15" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1334,16 +1323,16 @@
         <v>52</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>
       </c>
       <c r="D16" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E16" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="F16" t="s">
         <v>10</v>
@@ -1354,13 +1343,13 @@
         <v>53</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C17" t="s">
         <v>7</v>
       </c>
       <c r="D17" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E17" t="s">
         <v>9</v>
@@ -1374,13 +1363,13 @@
         <v>54</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C18" t="s">
         <v>7</v>
       </c>
       <c r="D18" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E18" t="s">
         <v>9</v>
@@ -1394,13 +1383,13 @@
         <v>55</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C19" t="s">
         <v>7</v>
       </c>
       <c r="D19" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E19" t="s">
         <v>9</v>
@@ -1414,13 +1403,13 @@
         <v>56</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C20" t="s">
         <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E20" t="s">
         <v>9</v>
@@ -1430,50 +1419,38 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>57</v>
-      </c>
-      <c r="B21" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" t="s">
-        <v>38</v>
-      </c>
-      <c r="E21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" t="s">
-        <v>10</v>
-      </c>
+      <c r="A21"/>
+      <c r="B21"/>
+      <c r="C21"/>
+      <c r="D21"/>
+      <c r="E21"/>
+      <c r="F21"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="39.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="37.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="47" style="2" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18" style="2" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="9.140625" style="2" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="2" width="7.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="39.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="16.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="37.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="2" width="47.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="2" width="18.0" collapsed="true"/>
+    <col min="7" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row ht="45" r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1494,8 +1471,8 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>1</v>
+      <c r="A2" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -1518,13 +1495,13 @@
         <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -1538,16 +1515,16 @@
         <v>40</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F4" t="s">
         <v>10</v>
@@ -1558,7 +1535,7 @@
         <v>41</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -1578,16 +1555,16 @@
         <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F6" t="s">
         <v>10</v>
@@ -1598,16 +1575,16 @@
         <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="F7" t="s">
         <v>10</v>
@@ -1618,19 +1595,19 @@
         <v>44</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E8" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F8" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1758,19 +1735,19 @@
         <v>51</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E15" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F15" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1778,16 +1755,16 @@
         <v>52</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>
       </c>
       <c r="D16" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E16" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="F16" t="s">
         <v>10</v>
@@ -1798,13 +1775,13 @@
         <v>53</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C17" t="s">
         <v>7</v>
       </c>
       <c r="D17" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E17" t="s">
         <v>9</v>
@@ -1818,13 +1795,13 @@
         <v>54</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C18" t="s">
         <v>7</v>
       </c>
       <c r="D18" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E18" t="s">
         <v>9</v>
@@ -1838,13 +1815,13 @@
         <v>55</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C19" t="s">
         <v>7</v>
       </c>
       <c r="D19" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E19" t="s">
         <v>9</v>
@@ -1858,13 +1835,13 @@
         <v>56</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C20" t="s">
         <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E20" t="s">
         <v>9</v>
@@ -1874,26 +1851,14 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>57</v>
-      </c>
-      <c r="B21" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" t="s">
-        <v>38</v>
-      </c>
-      <c r="E21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" t="s">
-        <v>10</v>
-      </c>
+      <c r="A21"/>
+      <c r="B21"/>
+      <c r="C21"/>
+      <c r="D21"/>
+      <c r="E21"/>
+      <c r="F21"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>